<commit_message>
SPI Review part 2 (final review)
</commit_message>
<xml_diff>
--- a/01_raw_data/4.1_SOCS/raw/D4.1.Manual.Review.xlsx
+++ b/01_raw_data/4.1_SOCS/raw/D4.1.Manual.Review.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/zprinsloo_worldbank_org/Documents/spi/technical-work/SPI/01_raw_data/4.1_SOCS/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_F25DC773A252ABDACC1048D7B19A782C5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4824C0AA-3A1A-4895-9DC4-0B60825CF91D}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="11_F25DC773A252ABDACC1048D7B19A782C5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C74E6D4B-A4BC-42A9-B225-4B81DFB2991D}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="-100" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="468">
   <si>
     <t>iso3c</t>
   </si>
@@ -1411,13 +1411,32 @@
   </si>
   <si>
     <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>Pillar 4 (Labor force survey): Yes, a labor force survey for 2021 can be found here: https://ins-cameroun.cm/statistique/eesi3-phase-2-enquete-sur-le-secteur-informel-principaux-indicateurs-depliant/</t>
+  </si>
+  <si>
+    <t>Pillar 4 (Population census): Yes, 2024 Population and Housing census found here: https://www.statistics.gov.lk/Resource/en/Population/CPH_2024/CPH2024_Preliminary_Report.pdf</t>
+  </si>
+  <si>
+    <t>2017, 2018, 2019, 2020, 2021, 2022, 2023, 2024</t>
+  </si>
+  <si>
+    <t>Pillar 4 (Business census): Yes, business registry as of 2024
+Pillar 4 (Labor force survey): Yes, annual labor force survey since 2017</t>
+  </si>
+  <si>
+    <t>Yes, 2021 agricultural census is now included. FAO documentation here: https://openknowledge.fao.org/server/api/core/bitstreams/f4cb45cb-419d-4a0f-aceb-fef28cf9045f/content</t>
+  </si>
+  <si>
+    <t>Yes, MICS 2021/2022 can be found here: https://mics.unicef.org/surveys?display=card&amp;keys=benin and has been attributed to the year 2021.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1446,6 +1465,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1468,11 +1493,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1489,6 +1518,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1756,11 +1789,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="11" width="13.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -2150,9 +2187,13 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
+      <c r="I22" s="2">
+        <v>2021</v>
+      </c>
       <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
+      <c r="K22" s="4" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
@@ -2391,10 +2432,14 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
+      <c r="H36" s="2">
+        <v>2021</v>
+      </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
+      <c r="K36" s="2" t="s">
+        <v>462</v>
+      </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
@@ -3202,14 +3247,18 @@
         <v>181</v>
       </c>
       <c r="C83" s="2"/>
-      <c r="D83" s="2"/>
+      <c r="D83" s="2">
+        <v>2021</v>
+      </c>
       <c r="E83" s="2"/>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
       <c r="J83" s="2"/>
-      <c r="K83" s="2"/>
+      <c r="K83" s="2" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
@@ -3517,7 +3566,7 @@
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" ht="180" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>218</v>
       </c>
@@ -3526,13 +3575,19 @@
       </c>
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
-      <c r="E102" s="2"/>
+      <c r="E102" s="2">
+        <v>2024</v>
+      </c>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
-      <c r="H102" s="2"/>
+      <c r="H102" s="2" t="s">
+        <v>464</v>
+      </c>
       <c r="I102" s="2"/>
       <c r="J102" s="2"/>
-      <c r="K102" s="2"/>
+      <c r="K102" s="5" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
@@ -4930,7 +4985,9 @@
       <c r="B182" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="C182" s="2"/>
+      <c r="C182" s="2">
+        <v>2024</v>
+      </c>
       <c r="D182" s="2"/>
       <c r="E182" s="2"/>
       <c r="F182" s="2"/>
@@ -4938,7 +4995,9 @@
       <c r="H182" s="2"/>
       <c r="I182" s="2"/>
       <c r="J182" s="2"/>
-      <c r="K182" s="2"/>
+      <c r="K182" s="2" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
@@ -5580,6 +5639,7 @@
     <hyperlink ref="K177" r:id="rId2" location="doc_desc.title_statement and https://sdd.spc.int/digital_library/solomon-islands-demographic-and-health-survey-dhs-2015" display="https://statistics.gov.sb/sinso-releases-national-economic-establishment-census-report-neec-2024/ and https:/microdata.pacificdata.org/index.php/catalog/482 - doc_desc.title_statement and https://sdd.spc.int/digital_library/solomon-islands-demographic-and-health-survey-dhs-2015" xr:uid="{382E6075-6F68-42E6-8073-BE325E02EA93}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <headerFooter>
     <oddFooter>&amp;R_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Official Use Only</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
post update revisions - SL SAU
</commit_message>
<xml_diff>
--- a/01_raw_data/4.1_SOCS/raw/D4.1.Manual.Review.xlsx
+++ b/01_raw_data/4.1_SOCS/raw/D4.1.Manual.Review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldbankgroup-my.sharepoint.com/personal/zprinsloo_worldbank_org/Documents/spi/technical-work/SPI/01_raw_data/4.1_SOCS/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="11_F25DC773A252ABDACC1048D7B19A782C5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C74E6D4B-A4BC-42A9-B225-4B81DFB2991D}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="11_F25DC773A252ABDACC1048D7B19A782C5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67F77C94-AFEC-4695-A871-AEF41C941A33}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-100" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="53880" yWindow="360" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1416,9 +1416,6 @@
     <t>Pillar 4 (Labor force survey): Yes, a labor force survey for 2021 can be found here: https://ins-cameroun.cm/statistique/eesi3-phase-2-enquete-sur-le-secteur-informel-principaux-indicateurs-depliant/</t>
   </si>
   <si>
-    <t>Pillar 4 (Population census): Yes, 2024 Population and Housing census found here: https://www.statistics.gov.lk/Resource/en/Population/CPH_2024/CPH2024_Preliminary_Report.pdf</t>
-  </si>
-  <si>
     <t>2017, 2018, 2019, 2020, 2021, 2022, 2023, 2024</t>
   </si>
   <si>
@@ -1430,6 +1427,10 @@
   </si>
   <si>
     <t>Yes, MICS 2021/2022 can be found here: https://mics.unicef.org/surveys?display=card&amp;keys=benin and has been attributed to the year 2021.</t>
+  </si>
+  <si>
+    <t>Pillar 4 (Population census): Yes, 2024 Population and Housing census found here: https://www.statistics.gov.lk/Resource/en/Population/CPH_2024/CPH2024_Preliminary_Report.pdf
+Pillar 4 (Dem/Health survey): Yes, 2016 DHS survey found here: https://www.statistics.gov.lk/Resource/en/Health/DemographicAndHealthSurveyReport-2016-Contents.pdf</t>
   </si>
 </sst>
 </file>
@@ -1493,13 +1494,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1790,16 +1794,16 @@
   <dimension ref="A1:K218"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
+      <pane ySplit="1" topLeftCell="A181" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K183" sqref="K183"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="11" width="13.85546875" customWidth="1"/>
+    <col min="1" max="11" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1834,7 +1838,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
@@ -1851,7 +1855,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
@@ -1868,7 +1872,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -1885,7 +1889,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -1902,7 +1906,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
@@ -1919,7 +1923,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -1936,7 +1940,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
@@ -1953,7 +1957,7 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
@@ -1970,7 +1974,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
@@ -1987,7 +1991,7 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>29</v>
       </c>
@@ -2004,7 +2008,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>31</v>
       </c>
@@ -2021,7 +2025,7 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>33</v>
       </c>
@@ -2038,7 +2042,7 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
@@ -2055,7 +2059,7 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>37</v>
       </c>
@@ -2072,7 +2076,7 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
@@ -2089,7 +2093,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>41</v>
       </c>
@@ -2106,7 +2110,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>43</v>
       </c>
@@ -2123,7 +2127,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>45</v>
       </c>
@@ -2140,7 +2144,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>47</v>
       </c>
@@ -2157,7 +2161,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>49</v>
       </c>
@@ -2174,7 +2178,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>51</v>
       </c>
@@ -2192,10 +2196,10 @@
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="4" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>53</v>
       </c>
@@ -2212,7 +2216,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>55</v>
       </c>
@@ -2229,7 +2233,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>57</v>
       </c>
@@ -2246,7 +2250,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>59</v>
       </c>
@@ -2263,7 +2267,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>61</v>
       </c>
@@ -2284,7 +2288,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>65</v>
       </c>
@@ -2301,7 +2305,7 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>67</v>
       </c>
@@ -2318,7 +2322,7 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>69</v>
       </c>
@@ -2335,7 +2339,7 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>71</v>
       </c>
@@ -2352,7 +2356,7 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>73</v>
       </c>
@@ -2369,7 +2373,7 @@
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>75</v>
       </c>
@@ -2386,7 +2390,7 @@
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>77</v>
       </c>
@@ -2403,7 +2407,7 @@
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>79</v>
       </c>
@@ -2420,7 +2424,7 @@
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>81</v>
       </c>
@@ -2441,7 +2445,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>83</v>
       </c>
@@ -2458,7 +2462,7 @@
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>85</v>
       </c>
@@ -2475,7 +2479,7 @@
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>87</v>
       </c>
@@ -2492,7 +2496,7 @@
       <c r="J39" s="2"/>
       <c r="K39" s="2"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>89</v>
       </c>
@@ -2509,7 +2513,7 @@
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>91</v>
       </c>
@@ -2526,7 +2530,7 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>93</v>
       </c>
@@ -2543,7 +2547,7 @@
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>95</v>
       </c>
@@ -2560,7 +2564,7 @@
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>97</v>
       </c>
@@ -2577,7 +2581,7 @@
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>99</v>
       </c>
@@ -2594,7 +2598,7 @@
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>101</v>
       </c>
@@ -2611,7 +2615,7 @@
       <c r="J46" s="2"/>
       <c r="K46" s="2"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>103</v>
       </c>
@@ -2628,7 +2632,7 @@
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>105</v>
       </c>
@@ -2645,7 +2649,7 @@
       <c r="J48" s="2"/>
       <c r="K48" s="2"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>107</v>
       </c>
@@ -2662,7 +2666,7 @@
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>109</v>
       </c>
@@ -2679,7 +2683,7 @@
       <c r="J50" s="2"/>
       <c r="K50" s="2"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>111</v>
       </c>
@@ -2696,7 +2700,7 @@
       <c r="J51" s="2"/>
       <c r="K51" s="2"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>113</v>
       </c>
@@ -2713,7 +2717,7 @@
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>115</v>
       </c>
@@ -2730,7 +2734,7 @@
       <c r="J53" s="2"/>
       <c r="K53" s="2"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>117</v>
       </c>
@@ -2747,7 +2751,7 @@
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>119</v>
       </c>
@@ -2764,7 +2768,7 @@
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>121</v>
       </c>
@@ -2781,7 +2785,7 @@
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>123</v>
       </c>
@@ -2798,7 +2802,7 @@
       <c r="J57" s="2"/>
       <c r="K57" s="2"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>125</v>
       </c>
@@ -2815,7 +2819,7 @@
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
         <v>127</v>
       </c>
@@ -2836,7 +2840,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>130</v>
       </c>
@@ -2853,7 +2857,7 @@
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>132</v>
       </c>
@@ -2870,7 +2874,7 @@
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>134</v>
       </c>
@@ -2887,7 +2891,7 @@
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>136</v>
       </c>
@@ -2904,7 +2908,7 @@
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>138</v>
       </c>
@@ -2921,7 +2925,7 @@
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>140</v>
       </c>
@@ -2938,7 +2942,7 @@
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>142</v>
       </c>
@@ -2955,7 +2959,7 @@
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>144</v>
       </c>
@@ -2972,7 +2976,7 @@
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>146</v>
       </c>
@@ -2997,7 +3001,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>151</v>
       </c>
@@ -3014,7 +3018,7 @@
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>153</v>
       </c>
@@ -3031,7 +3035,7 @@
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>155</v>
       </c>
@@ -3048,7 +3052,7 @@
       <c r="J71" s="2"/>
       <c r="K71" s="2"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>157</v>
       </c>
@@ -3065,7 +3069,7 @@
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>159</v>
       </c>
@@ -3086,7 +3090,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>162</v>
       </c>
@@ -3103,7 +3107,7 @@
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
         <v>164</v>
       </c>
@@ -3120,7 +3124,7 @@
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>166</v>
       </c>
@@ -3137,7 +3141,7 @@
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A77" s="2" t="s">
         <v>168</v>
       </c>
@@ -3154,7 +3158,7 @@
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>170</v>
       </c>
@@ -3171,7 +3175,7 @@
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A79" s="2" t="s">
         <v>172</v>
       </c>
@@ -3188,7 +3192,7 @@
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>174</v>
       </c>
@@ -3205,7 +3209,7 @@
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
         <v>176</v>
       </c>
@@ -3222,7 +3226,7 @@
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
         <v>178</v>
       </c>
@@ -3239,7 +3243,7 @@
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" s="2" t="s">
         <v>180</v>
       </c>
@@ -3257,10 +3261,10 @@
       <c r="I83" s="2"/>
       <c r="J83" s="2"/>
       <c r="K83" s="2" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" s="2" t="s">
         <v>182</v>
       </c>
@@ -3277,7 +3281,7 @@
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" s="2" t="s">
         <v>184</v>
       </c>
@@ -3294,7 +3298,7 @@
       <c r="J85" s="2"/>
       <c r="K85" s="2"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
         <v>186</v>
       </c>
@@ -3311,7 +3315,7 @@
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
         <v>188</v>
       </c>
@@ -3328,7 +3332,7 @@
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
         <v>190</v>
       </c>
@@ -3345,7 +3349,7 @@
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89" s="2" t="s">
         <v>192</v>
       </c>
@@ -3362,7 +3366,7 @@
       <c r="J89" s="2"/>
       <c r="K89" s="2"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
         <v>194</v>
       </c>
@@ -3379,7 +3383,7 @@
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91" s="2" t="s">
         <v>196</v>
       </c>
@@ -3396,7 +3400,7 @@
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="s">
         <v>198</v>
       </c>
@@ -3413,7 +3417,7 @@
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
         <v>200</v>
       </c>
@@ -3430,7 +3434,7 @@
       <c r="J93" s="2"/>
       <c r="K93" s="2"/>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
         <v>202</v>
       </c>
@@ -3447,7 +3451,7 @@
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95" s="2" t="s">
         <v>204</v>
       </c>
@@ -3464,7 +3468,7 @@
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
         <v>206</v>
       </c>
@@ -3481,7 +3485,7 @@
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
         <v>208</v>
       </c>
@@ -3498,7 +3502,7 @@
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
         <v>210</v>
       </c>
@@ -3515,7 +3519,7 @@
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99" s="2" t="s">
         <v>212</v>
       </c>
@@ -3532,7 +3536,7 @@
       <c r="J99" s="2"/>
       <c r="K99" s="2"/>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="s">
         <v>214</v>
       </c>
@@ -3549,7 +3553,7 @@
       <c r="J100" s="2"/>
       <c r="K100" s="2"/>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A101" s="2" t="s">
         <v>216</v>
       </c>
@@ -3566,7 +3570,7 @@
       <c r="J101" s="2"/>
       <c r="K101" s="2"/>
     </row>
-    <row r="102" spans="1:11" ht="180" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" ht="174" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
         <v>218</v>
       </c>
@@ -3581,15 +3585,15 @@
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
       <c r="H102" s="2" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I102" s="2"/>
       <c r="J102" s="2"/>
       <c r="K102" s="5" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
         <v>220</v>
       </c>
@@ -3606,7 +3610,7 @@
       <c r="J103" s="2"/>
       <c r="K103" s="2"/>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
         <v>222</v>
       </c>
@@ -3629,7 +3633,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A105" s="2" t="s">
         <v>225</v>
       </c>
@@ -3646,7 +3650,7 @@
       <c r="J105" s="2"/>
       <c r="K105" s="2"/>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
         <v>227</v>
       </c>
@@ -3663,7 +3667,7 @@
       <c r="J106" s="2"/>
       <c r="K106" s="2"/>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
         <v>229</v>
       </c>
@@ -3680,7 +3684,7 @@
       <c r="J107" s="2"/>
       <c r="K107" s="2"/>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A108" s="2" t="s">
         <v>231</v>
       </c>
@@ -3697,7 +3701,7 @@
       <c r="J108" s="2"/>
       <c r="K108" s="2"/>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A109" s="2" t="s">
         <v>233</v>
       </c>
@@ -3714,7 +3718,7 @@
       <c r="J109" s="2"/>
       <c r="K109" s="2"/>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A110" s="2" t="s">
         <v>235</v>
       </c>
@@ -3731,7 +3735,7 @@
       <c r="J110" s="2"/>
       <c r="K110" s="2"/>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A111" s="2" t="s">
         <v>237</v>
       </c>
@@ -3748,7 +3752,7 @@
       <c r="J111" s="2"/>
       <c r="K111" s="2"/>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A112" s="2" t="s">
         <v>239</v>
       </c>
@@ -3765,7 +3769,7 @@
       <c r="J112" s="2"/>
       <c r="K112" s="2"/>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A113" s="2" t="s">
         <v>241</v>
       </c>
@@ -3782,7 +3786,7 @@
       <c r="J113" s="2"/>
       <c r="K113" s="2"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A114" s="2" t="s">
         <v>243</v>
       </c>
@@ -3805,7 +3809,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A115" s="2" t="s">
         <v>246</v>
       </c>
@@ -3822,7 +3826,7 @@
       <c r="J115" s="2"/>
       <c r="K115" s="2"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A116" s="2" t="s">
         <v>248</v>
       </c>
@@ -3839,7 +3843,7 @@
       <c r="J116" s="2"/>
       <c r="K116" s="2"/>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A117" s="2" t="s">
         <v>250</v>
       </c>
@@ -3856,7 +3860,7 @@
       <c r="J117" s="2"/>
       <c r="K117" s="2"/>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A118" s="2" t="s">
         <v>252</v>
       </c>
@@ -3873,7 +3877,7 @@
       <c r="J118" s="2"/>
       <c r="K118" s="2"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A119" s="2" t="s">
         <v>254</v>
       </c>
@@ -3890,7 +3894,7 @@
       <c r="J119" s="2"/>
       <c r="K119" s="2"/>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="s">
         <v>256</v>
       </c>
@@ -3907,7 +3911,7 @@
       <c r="J120" s="2"/>
       <c r="K120" s="2"/>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A121" s="2" t="s">
         <v>258</v>
       </c>
@@ -3924,7 +3928,7 @@
       <c r="J121" s="2"/>
       <c r="K121" s="2"/>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A122" s="2" t="s">
         <v>260</v>
       </c>
@@ -3941,7 +3945,7 @@
       <c r="J122" s="2"/>
       <c r="K122" s="2"/>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A123" s="2" t="s">
         <v>262</v>
       </c>
@@ -3958,7 +3962,7 @@
       <c r="J123" s="2"/>
       <c r="K123" s="2"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A124" s="2" t="s">
         <v>264</v>
       </c>
@@ -3975,7 +3979,7 @@
       <c r="J124" s="2"/>
       <c r="K124" s="2"/>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A125" s="2" t="s">
         <v>266</v>
       </c>
@@ -3992,7 +3996,7 @@
       <c r="J125" s="2"/>
       <c r="K125" s="2"/>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A126" s="2" t="s">
         <v>268</v>
       </c>
@@ -4009,7 +4013,7 @@
       <c r="J126" s="2"/>
       <c r="K126" s="2"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
         <v>270</v>
       </c>
@@ -4026,7 +4030,7 @@
       <c r="J127" s="2"/>
       <c r="K127" s="2"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A128" s="2" t="s">
         <v>272</v>
       </c>
@@ -4043,7 +4047,7 @@
       <c r="J128" s="2"/>
       <c r="K128" s="2"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A129" s="2" t="s">
         <v>274</v>
       </c>
@@ -4060,7 +4064,7 @@
       <c r="J129" s="2"/>
       <c r="K129" s="2"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A130" s="2" t="s">
         <v>276</v>
       </c>
@@ -4077,7 +4081,7 @@
       <c r="J130" s="2"/>
       <c r="K130" s="2"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A131" s="2" t="s">
         <v>278</v>
       </c>
@@ -4094,7 +4098,7 @@
       <c r="J131" s="2"/>
       <c r="K131" s="2"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A132" s="2" t="s">
         <v>280</v>
       </c>
@@ -4111,7 +4115,7 @@
       <c r="J132" s="2"/>
       <c r="K132" s="2"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A133" s="2" t="s">
         <v>282</v>
       </c>
@@ -4128,7 +4132,7 @@
       <c r="J133" s="2"/>
       <c r="K133" s="2"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="s">
         <v>284</v>
       </c>
@@ -4145,7 +4149,7 @@
       <c r="J134" s="2"/>
       <c r="K134" s="2"/>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="s">
         <v>286</v>
       </c>
@@ -4162,7 +4166,7 @@
       <c r="J135" s="2"/>
       <c r="K135" s="2"/>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A136" s="2" t="s">
         <v>288</v>
       </c>
@@ -4179,7 +4183,7 @@
       <c r="J136" s="2"/>
       <c r="K136" s="2"/>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A137" s="2" t="s">
         <v>290</v>
       </c>
@@ -4196,7 +4200,7 @@
       <c r="J137" s="2"/>
       <c r="K137" s="2"/>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A138" s="2" t="s">
         <v>292</v>
       </c>
@@ -4213,7 +4217,7 @@
       <c r="J138" s="2"/>
       <c r="K138" s="2"/>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A139" s="2" t="s">
         <v>294</v>
       </c>
@@ -4234,7 +4238,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A140" s="2" t="s">
         <v>297</v>
       </c>
@@ -4251,7 +4255,7 @@
       <c r="J140" s="2"/>
       <c r="K140" s="2"/>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A141" s="2" t="s">
         <v>299</v>
       </c>
@@ -4268,7 +4272,7 @@
       <c r="J141" s="2"/>
       <c r="K141" s="2"/>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A142" s="2" t="s">
         <v>301</v>
       </c>
@@ -4285,7 +4289,7 @@
       <c r="J142" s="2"/>
       <c r="K142" s="2"/>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A143" s="2" t="s">
         <v>303</v>
       </c>
@@ -4302,7 +4306,7 @@
       <c r="J143" s="2"/>
       <c r="K143" s="2"/>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A144" s="2" t="s">
         <v>305</v>
       </c>
@@ -4319,7 +4323,7 @@
       <c r="J144" s="2"/>
       <c r="K144" s="2"/>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A145" s="2" t="s">
         <v>307</v>
       </c>
@@ -4336,7 +4340,7 @@
       <c r="J145" s="2"/>
       <c r="K145" s="2"/>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A146" s="2" t="s">
         <v>309</v>
       </c>
@@ -4353,7 +4357,7 @@
       <c r="J146" s="2"/>
       <c r="K146" s="2"/>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A147" s="2" t="s">
         <v>311</v>
       </c>
@@ -4370,7 +4374,7 @@
       <c r="J147" s="2"/>
       <c r="K147" s="2"/>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A148" s="2" t="s">
         <v>313</v>
       </c>
@@ -4387,7 +4391,7 @@
       <c r="J148" s="2"/>
       <c r="K148" s="2"/>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A149" s="2" t="s">
         <v>315</v>
       </c>
@@ -4404,7 +4408,7 @@
       <c r="J149" s="2"/>
       <c r="K149" s="2"/>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A150" s="2" t="s">
         <v>317</v>
       </c>
@@ -4421,7 +4425,7 @@
       <c r="J150" s="2"/>
       <c r="K150" s="2"/>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A151" s="2" t="s">
         <v>319</v>
       </c>
@@ -4438,7 +4442,7 @@
       <c r="J151" s="2"/>
       <c r="K151" s="2"/>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A152" s="2" t="s">
         <v>321</v>
       </c>
@@ -4455,7 +4459,7 @@
       <c r="J152" s="2"/>
       <c r="K152" s="2"/>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A153" s="2" t="s">
         <v>323</v>
       </c>
@@ -4472,7 +4476,7 @@
       <c r="J153" s="2"/>
       <c r="K153" s="2"/>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A154" s="2" t="s">
         <v>325</v>
       </c>
@@ -4489,7 +4493,7 @@
       <c r="J154" s="2"/>
       <c r="K154" s="2"/>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A155" s="2" t="s">
         <v>327</v>
       </c>
@@ -4506,7 +4510,7 @@
       <c r="J155" s="2"/>
       <c r="K155" s="2"/>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A156" s="2" t="s">
         <v>329</v>
       </c>
@@ -4523,7 +4527,7 @@
       <c r="J156" s="2"/>
       <c r="K156" s="2"/>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A157" s="2" t="s">
         <v>331</v>
       </c>
@@ -4540,7 +4544,7 @@
       <c r="J157" s="2"/>
       <c r="K157" s="2"/>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A158" s="2" t="s">
         <v>333</v>
       </c>
@@ -4557,7 +4561,7 @@
       <c r="J158" s="2"/>
       <c r="K158" s="2"/>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A159" s="2" t="s">
         <v>335</v>
       </c>
@@ -4574,7 +4578,7 @@
       <c r="J159" s="2"/>
       <c r="K159" s="2"/>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A160" s="2" t="s">
         <v>337</v>
       </c>
@@ -4591,7 +4595,7 @@
       <c r="J160" s="2"/>
       <c r="K160" s="2"/>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A161" s="2" t="s">
         <v>339</v>
       </c>
@@ -4608,7 +4612,7 @@
       <c r="J161" s="2"/>
       <c r="K161" s="2"/>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A162" s="2" t="s">
         <v>341</v>
       </c>
@@ -4625,7 +4629,7 @@
       <c r="J162" s="2"/>
       <c r="K162" s="2"/>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A163" s="2" t="s">
         <v>343</v>
       </c>
@@ -4642,7 +4646,7 @@
       <c r="J163" s="2"/>
       <c r="K163" s="2"/>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A164" s="2" t="s">
         <v>345</v>
       </c>
@@ -4659,7 +4663,7 @@
       <c r="J164" s="2"/>
       <c r="K164" s="2"/>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A165" s="2" t="s">
         <v>347</v>
       </c>
@@ -4684,7 +4688,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A166" s="2" t="s">
         <v>350</v>
       </c>
@@ -4701,7 +4705,7 @@
       <c r="J166" s="2"/>
       <c r="K166" s="2"/>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A167" s="2" t="s">
         <v>352</v>
       </c>
@@ -4718,7 +4722,7 @@
       <c r="J167" s="2"/>
       <c r="K167" s="2"/>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A168" s="2" t="s">
         <v>354</v>
       </c>
@@ -4741,7 +4745,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A169" s="2" t="s">
         <v>357</v>
       </c>
@@ -4758,7 +4762,7 @@
       <c r="J169" s="2"/>
       <c r="K169" s="2"/>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A170" s="2" t="s">
         <v>359</v>
       </c>
@@ -4775,7 +4779,7 @@
       <c r="J170" s="2"/>
       <c r="K170" s="2"/>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A171" s="2" t="s">
         <v>361</v>
       </c>
@@ -4792,7 +4796,7 @@
       <c r="J171" s="2"/>
       <c r="K171" s="2"/>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A172" s="2" t="s">
         <v>363</v>
       </c>
@@ -4809,7 +4813,7 @@
       <c r="J172" s="2"/>
       <c r="K172" s="2"/>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A173" s="2" t="s">
         <v>365</v>
       </c>
@@ -4826,7 +4830,7 @@
       <c r="J173" s="2"/>
       <c r="K173" s="2"/>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A174" s="2" t="s">
         <v>367</v>
       </c>
@@ -4843,7 +4847,7 @@
       <c r="J174" s="2"/>
       <c r="K174" s="2"/>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A175" s="2" t="s">
         <v>369</v>
       </c>
@@ -4860,7 +4864,7 @@
       <c r="J175" s="2"/>
       <c r="K175" s="2"/>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A176" s="2" t="s">
         <v>371</v>
       </c>
@@ -4877,7 +4881,7 @@
       <c r="J176" s="2"/>
       <c r="K176" s="2"/>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A177" s="2" t="s">
         <v>373</v>
       </c>
@@ -4902,7 +4906,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A178" s="2" t="s">
         <v>376</v>
       </c>
@@ -4927,7 +4931,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A179" s="2" t="s">
         <v>379</v>
       </c>
@@ -4944,7 +4948,7 @@
       <c r="J179" s="2"/>
       <c r="K179" s="2"/>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A180" s="2" t="s">
         <v>381</v>
       </c>
@@ -4961,7 +4965,7 @@
       <c r="J180" s="2"/>
       <c r="K180" s="2"/>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A181" s="2" t="s">
         <v>383</v>
       </c>
@@ -4978,7 +4982,7 @@
       <c r="J181" s="2"/>
       <c r="K181" s="2"/>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:11" ht="406" x14ac:dyDescent="0.35">
       <c r="A182" s="2" t="s">
         <v>385</v>
       </c>
@@ -4993,13 +4997,15 @@
       <c r="F182" s="2"/>
       <c r="G182" s="2"/>
       <c r="H182" s="2"/>
-      <c r="I182" s="2"/>
+      <c r="I182" s="2">
+        <v>2016</v>
+      </c>
       <c r="J182" s="2"/>
-      <c r="K182" s="2" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K182" s="6" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A183" s="2" t="s">
         <v>387</v>
       </c>
@@ -5016,7 +5022,7 @@
       <c r="J183" s="2"/>
       <c r="K183" s="2"/>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A184" s="2" t="s">
         <v>389</v>
       </c>
@@ -5033,7 +5039,7 @@
       <c r="J184" s="2"/>
       <c r="K184" s="2"/>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A185" s="2" t="s">
         <v>391</v>
       </c>
@@ -5050,7 +5056,7 @@
       <c r="J185" s="2"/>
       <c r="K185" s="2"/>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A186" s="2" t="s">
         <v>393</v>
       </c>
@@ -5067,7 +5073,7 @@
       <c r="J186" s="2"/>
       <c r="K186" s="2"/>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A187" s="2" t="s">
         <v>395</v>
       </c>
@@ -5084,7 +5090,7 @@
       <c r="J187" s="2"/>
       <c r="K187" s="2"/>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A188" s="2" t="s">
         <v>397</v>
       </c>
@@ -5101,7 +5107,7 @@
       <c r="J188" s="2"/>
       <c r="K188" s="2"/>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A189" s="2" t="s">
         <v>399</v>
       </c>
@@ -5118,7 +5124,7 @@
       <c r="J189" s="2"/>
       <c r="K189" s="2"/>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A190" s="2" t="s">
         <v>401</v>
       </c>
@@ -5135,7 +5141,7 @@
       <c r="J190" s="2"/>
       <c r="K190" s="2"/>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A191" s="2" t="s">
         <v>403</v>
       </c>
@@ -5152,7 +5158,7 @@
       <c r="J191" s="2"/>
       <c r="K191" s="2"/>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A192" s="2" t="s">
         <v>405</v>
       </c>
@@ -5169,7 +5175,7 @@
       <c r="J192" s="2"/>
       <c r="K192" s="2"/>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A193" s="2" t="s">
         <v>407</v>
       </c>
@@ -5186,7 +5192,7 @@
       <c r="J193" s="2"/>
       <c r="K193" s="2"/>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A194" s="2" t="s">
         <v>409</v>
       </c>
@@ -5203,7 +5209,7 @@
       <c r="J194" s="2"/>
       <c r="K194" s="2"/>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A195" s="2" t="s">
         <v>411</v>
       </c>
@@ -5220,7 +5226,7 @@
       <c r="J195" s="2"/>
       <c r="K195" s="2"/>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A196" s="2" t="s">
         <v>413</v>
       </c>
@@ -5237,7 +5243,7 @@
       <c r="J196" s="2"/>
       <c r="K196" s="2"/>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A197" s="2" t="s">
         <v>415</v>
       </c>
@@ -5258,7 +5264,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A198" s="2" t="s">
         <v>418</v>
       </c>
@@ -5275,7 +5281,7 @@
       <c r="J198" s="2"/>
       <c r="K198" s="2"/>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A199" s="2" t="s">
         <v>420</v>
       </c>
@@ -5292,7 +5298,7 @@
       <c r="J199" s="2"/>
       <c r="K199" s="2"/>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A200" s="2" t="s">
         <v>422</v>
       </c>
@@ -5309,7 +5315,7 @@
       <c r="J200" s="2"/>
       <c r="K200" s="2"/>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A201" s="2" t="s">
         <v>424</v>
       </c>
@@ -5326,7 +5332,7 @@
       <c r="J201" s="2"/>
       <c r="K201" s="2"/>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A202" s="2" t="s">
         <v>426</v>
       </c>
@@ -5343,7 +5349,7 @@
       <c r="J202" s="2"/>
       <c r="K202" s="2"/>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A203" s="2" t="s">
         <v>428</v>
       </c>
@@ -5366,7 +5372,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A204" s="2" t="s">
         <v>431</v>
       </c>
@@ -5383,7 +5389,7 @@
       <c r="J204" s="2"/>
       <c r="K204" s="2"/>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A205" s="2" t="s">
         <v>433</v>
       </c>
@@ -5400,7 +5406,7 @@
       <c r="J205" s="2"/>
       <c r="K205" s="2"/>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A206" s="2" t="s">
         <v>435</v>
       </c>
@@ -5417,7 +5423,7 @@
       <c r="J206" s="2"/>
       <c r="K206" s="2"/>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A207" s="2" t="s">
         <v>437</v>
       </c>
@@ -5434,7 +5440,7 @@
       <c r="J207" s="2"/>
       <c r="K207" s="2"/>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A208" s="2" t="s">
         <v>439</v>
       </c>
@@ -5451,7 +5457,7 @@
       <c r="J208" s="2"/>
       <c r="K208" s="2"/>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A209" s="2" t="s">
         <v>441</v>
       </c>
@@ -5468,7 +5474,7 @@
       <c r="J209" s="2"/>
       <c r="K209" s="2"/>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A210" s="2" t="s">
         <v>443</v>
       </c>
@@ -5485,7 +5491,7 @@
       <c r="J210" s="2"/>
       <c r="K210" s="2"/>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A211" s="2" t="s">
         <v>445</v>
       </c>
@@ -5514,7 +5520,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A212" s="2" t="s">
         <v>448</v>
       </c>
@@ -5531,7 +5537,7 @@
       <c r="J212" s="2"/>
       <c r="K212" s="2"/>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A213" s="2" t="s">
         <v>450</v>
       </c>
@@ -5548,7 +5554,7 @@
       <c r="J213" s="2"/>
       <c r="K213" s="2"/>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A214" s="2" t="s">
         <v>452</v>
       </c>
@@ -5565,7 +5571,7 @@
       <c r="J214" s="2"/>
       <c r="K214" s="2"/>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A215" s="2" t="s">
         <v>454</v>
       </c>
@@ -5582,7 +5588,7 @@
       <c r="J215" s="2"/>
       <c r="K215" s="2"/>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A216" s="2" t="s">
         <v>456</v>
       </c>
@@ -5599,7 +5605,7 @@
       <c r="J216" s="2"/>
       <c r="K216" s="2"/>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A217" s="2" t="s">
         <v>458</v>
       </c>
@@ -5616,7 +5622,7 @@
       <c r="J217" s="2"/>
       <c r="K217" s="2"/>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A218" s="2" t="s">
         <v>460</v>
       </c>

</xml_diff>